<commit_message>
adding a format for each file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t xml:space="preserve">file name </t>
   </si>
@@ -37,6 +37,72 @@
     <t xml:space="preserve">number of issues : </t>
   </si>
   <si>
+    <t>unresolved issues</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>aarouche2016@gmail.com</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>MAJOR</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>CODE_SMELL</t>
+  </si>
+  <si>
+    <t>Creation Date</t>
+  </si>
+  <si>
+    <t>2022-03-17T12:06:21+0100</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Value stored to 'num' during its initialization is never read</t>
+  </si>
+  <si>
+    <t>Fixed issues</t>
+  </si>
+  <si>
+    <t>geoffray.adde@sonarsource.com</t>
+  </si>
+  <si>
+    <t>MINOR</t>
+  </si>
+  <si>
+    <t>2020-02-03T18:08:43+0100</t>
+  </si>
+  <si>
+    <t>Use the init-statement to declare "num" inside the if statement.</t>
+  </si>
+  <si>
+    <t>BUG</t>
+  </si>
+  <si>
+    <t>This branch can not be reached because the condition duplicates a previous condition in the same sequence of "if/else if" statements</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>Use the "nullptr" literal.</t>
+  </si>
+  <si>
+    <t>Remove this empty statement.</t>
+  </si>
+  <si>
     <t>hello.cpp</t>
   </si>
   <si>
@@ -46,6 +112,12 @@
     <t>AX-XYzyh4htFjYcVApkp</t>
   </si>
   <si>
+    <t>2022-03-17T11:18:20+0100</t>
+  </si>
+  <si>
+    <t>Remove this using-directive.</t>
+  </si>
+  <si>
     <t>test_debug_branch.cpp</t>
   </si>
   <si>
@@ -53,6 +125,9 @@
   </si>
   <si>
     <t>AX-Xhzcv9bpcrwAK8Imx</t>
+  </si>
+  <si>
+    <t>2022-03-17T11:57:59+0100</t>
   </si>
 </sst>
 </file>
@@ -68,15 +143,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -84,12 +171,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,93 +495,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="42.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="K6:L6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>